<commit_message>
Add local area density vs potential radius plots
</commit_message>
<xml_diff>
--- a/MySEProject/Dataset Reports/Dataset-GurunagSai/LocalAreaDensity vs PotentialRadius.xlsx
+++ b/MySEProject/Dataset Reports/Dataset-GurunagSai/LocalAreaDensity vs PotentialRadius.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\MySEProject\Dataset Reports\Dataset-GurunagSai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01492C98-3F17-4DC1-A8E7-E997910E83B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F14CC7E-83EC-4678-8475-F241E28683AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,22 +36,6 @@
     <t>Input similarities between two images</t>
   </si>
   <si>
-    <t>rectangle0_rectangle_2
-output similarity</t>
-  </si>
-  <si>
-    <t>rectangle0__triangle0
-output similarity</t>
-  </si>
-  <si>
-    <t>rectangle0_rectangle_2
-input similarity</t>
-  </si>
-  <si>
-    <t>rectangle0__triangle0
-Input Similarity</t>
-  </si>
-  <si>
     <t>Potential Radius</t>
   </si>
   <si>
@@ -74,6 +58,22 @@
   </si>
   <si>
     <t>Potential Radius = 1</t>
+  </si>
+  <si>
+    <t>rectangle00_rectangle_02
+input similarity</t>
+  </si>
+  <si>
+    <t>rectangle00__triangle00
+Input Similarity</t>
+  </si>
+  <si>
+    <t>rectangle00_rectangle_02
+output similarity</t>
+  </si>
+  <si>
+    <t>rectangle00__triangle00
+output similarity</t>
   </si>
 </sst>
 </file>
@@ -205,7 +205,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Output Similarity Between Rectangle0 &amp; Rectangle2</a:t>
+              <a:t>Output Similarity Between Rectangle00 &amp; Rectangle02</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1652,14 +1652,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>5562600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>78</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>699861</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
       <xdr:row>100</xdr:row>
       <xdr:rowOff>56697</xdr:rowOff>
     </xdr:to>
@@ -1995,26 +1995,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="23.28515625" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -2023,25 +2023,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2222,7 +2222,7 @@
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2403,7 +2403,7 @@
     </row>
     <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2584,7 +2584,7 @@
     </row>
     <row r="36" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2765,7 +2765,7 @@
     </row>
     <row r="47" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2946,7 +2946,7 @@
     </row>
     <row r="58" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>